<commit_message>
Implementation aller retour request
</commit_message>
<xml_diff>
--- a/BN.xlsx
+++ b/BN.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LS4Tonio\IN'TECH_INFO\Fonctionnel\Bataille Navale\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_iti\programmationFonctionnelle\BatailleNavale\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>User</t>
   </si>
@@ -62,9 +62,6 @@
     <t>LengthY</t>
   </si>
   <si>
-    <t>Cells</t>
-  </si>
-  <si>
     <t>Cell</t>
   </si>
   <si>
@@ -122,7 +119,13 @@
     <t>NumberHit</t>
   </si>
   <si>
-    <t>CellState</t>
+    <t>Lines</t>
+  </si>
+  <si>
+    <t>Line</t>
+  </si>
+  <si>
+    <t>cells</t>
   </si>
 </sst>
 </file>
@@ -569,46 +572,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>0</v>
@@ -620,7 +623,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>2</v>
@@ -629,18 +632,18 @@
         <v>1</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>7</v>
@@ -658,10 +661,10 @@
         <v>7</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -671,7 +674,7 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="3" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -679,15 +682,15 @@
         <v>8</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -699,12 +702,12 @@
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -715,7 +718,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -723,7 +726,17 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D9" s="6" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>